<commit_message>
Updated source files to version 1.0.1
</commit_message>
<xml_diff>
--- a/display-fw/TouchGFX/assets/texts/texts.xlsx
+++ b/display-fw/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23516" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24949" uniqueCount="298">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1047,6 +1047,21 @@
   <si>
     <t xml:space="preserve">Selftest in progress...
 This will take few minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooling System:  &lt;value&gt;° &lt;value&gt;     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: 1.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text_graph_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooling System:  &lt;value&gt;°&lt;value&gt;     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-., 0123456789CF</t>
   </si>
 </sst>
 </file>
@@ -2449,6 +2464,27 @@
       <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16">
+      <c r="B9" t="s">
+        <v>295</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>297</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
       <c r="L9" s="11" t="s">
         <v>6</v>
       </c>
@@ -2620,7 +2656,7 @@
         <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>295</v>
       </c>
       <c r="D8" t="s">
         <v>43</v>
@@ -2629,12 +2665,12 @@
         <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
         <v>71</v>
@@ -2646,12 +2682,12 @@
         <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
         <v>71</v>
@@ -2663,29 +2699,29 @@
         <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
         <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>179</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
@@ -2702,7 +2738,7 @@
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
@@ -2719,24 +2755,24 @@
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>148</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
         <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
         <v>148</v>
@@ -2748,12 +2784,12 @@
         <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
         <v>148</v>
@@ -2765,12 +2801,12 @@
         <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C17" t="s">
         <v>148</v>
@@ -2782,15 +2818,15 @@
         <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C18" t="s">
-        <v>148</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
         <v>43</v>
@@ -2799,12 +2835,12 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
@@ -2816,15 +2852,15 @@
         <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
         <v>43</v>
@@ -2833,12 +2869,12 @@
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>141</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="C21" t="s">
         <v>71</v>
@@ -2850,12 +2886,12 @@
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C22" t="s">
         <v>71</v>
@@ -2872,10 +2908,10 @@
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
         <v>43</v>
@@ -2884,15 +2920,15 @@
         <v>44</v>
       </c>
       <c r="F23" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>295</v>
       </c>
       <c r="D24" t="s">
         <v>43</v>
@@ -2901,32 +2937,32 @@
         <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
         <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>186</v>
+        <v>294</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
         <v>43</v>
@@ -2935,49 +2971,49 @@
         <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="C27" t="s">
         <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E27" t="s">
         <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>214</v>
+        <v>122</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E28" t="s">
         <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>186</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D29" t="s">
         <v>43</v>
@@ -2986,29 +3022,29 @@
         <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>184</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>122</v>
+        <v>228</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E30" t="s">
         <v>44</v>
       </c>
       <c r="F30" t="s">
-        <v>123</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
@@ -3020,12 +3056,12 @@
         <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C32" t="s">
         <v>71</v>
@@ -3037,15 +3073,15 @@
         <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>269</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
         <v>43</v>
@@ -3054,15 +3090,15 @@
         <v>44</v>
       </c>
       <c r="F33" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D34" t="s">
         <v>43</v>
@@ -3071,15 +3107,15 @@
         <v>44</v>
       </c>
       <c r="F34" t="s">
-        <v>230</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D35" t="s">
         <v>43</v>
@@ -3093,7 +3129,7 @@
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C36" t="s">
         <v>38</v>
@@ -3105,12 +3141,12 @@
         <v>44</v>
       </c>
       <c r="F36" t="s">
-        <v>57</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
@@ -3122,12 +3158,12 @@
         <v>44</v>
       </c>
       <c r="F37" t="s">
-        <v>57</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C38" t="s">
         <v>38</v>
@@ -3139,12 +3175,12 @@
         <v>44</v>
       </c>
       <c r="F38" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C39" t="s">
         <v>38</v>
@@ -3156,12 +3192,12 @@
         <v>44</v>
       </c>
       <c r="F39" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
@@ -3173,32 +3209,32 @@
         <v>44</v>
       </c>
       <c r="F40" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>242</v>
+        <v>182</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
+        <v>143</v>
       </c>
       <c r="E41" t="s">
         <v>44</v>
       </c>
       <c r="F41" t="s">
-        <v>243</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>244</v>
+        <v>180</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D42" t="s">
         <v>43</v>
@@ -3207,32 +3243,32 @@
         <v>44</v>
       </c>
       <c r="F42" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>182</v>
+        <v>246</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>143</v>
+        <v>50</v>
       </c>
       <c r="E43" t="s">
         <v>44</v>
       </c>
       <c r="F43" t="s">
-        <v>181</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>180</v>
+        <v>247</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D44" t="s">
         <v>43</v>
@@ -3241,32 +3277,32 @@
         <v>44</v>
       </c>
       <c r="F44" t="s">
-        <v>181</v>
+        <v>248</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E45" t="s">
         <v>44</v>
       </c>
       <c r="F45" t="s">
-        <v>123</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D46" t="s">
         <v>43</v>
@@ -3275,12 +3311,12 @@
         <v>44</v>
       </c>
       <c r="F46" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C47" t="s">
         <v>38</v>
@@ -3292,12 +3328,12 @@
         <v>44</v>
       </c>
       <c r="F47" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C48" t="s">
         <v>71</v>
@@ -3309,12 +3345,12 @@
         <v>44</v>
       </c>
       <c r="F48" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C49" t="s">
         <v>38</v>
@@ -3326,12 +3362,12 @@
         <v>44</v>
       </c>
       <c r="F49" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C50" t="s">
         <v>71</v>
@@ -3343,12 +3379,12 @@
         <v>44</v>
       </c>
       <c r="F50" t="s">
-        <v>290</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C51" t="s">
         <v>38</v>
@@ -3360,12 +3396,12 @@
         <v>44</v>
       </c>
       <c r="F51" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C52" t="s">
         <v>71</v>
@@ -3377,12 +3413,12 @@
         <v>44</v>
       </c>
       <c r="F52" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C53" t="s">
         <v>38</v>
@@ -3394,12 +3430,12 @@
         <v>44</v>
       </c>
       <c r="F53" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C54" t="s">
         <v>71</v>
@@ -3411,12 +3447,12 @@
         <v>44</v>
       </c>
       <c r="F54" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="C55" t="s">
         <v>38</v>
@@ -3428,15 +3464,15 @@
         <v>44</v>
       </c>
       <c r="F55" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="C56" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D56" t="s">
         <v>43</v>
@@ -3445,12 +3481,12 @@
         <v>44</v>
       </c>
       <c r="F56" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C57" t="s">
         <v>38</v>
@@ -3462,15 +3498,15 @@
         <v>44</v>
       </c>
       <c r="F57" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>272</v>
+        <v>89</v>
       </c>
       <c r="C58" t="s">
-        <v>38</v>
+        <v>295</v>
       </c>
       <c r="D58" t="s">
         <v>43</v>
@@ -3479,26 +3515,10 @@
         <v>44</v>
       </c>
       <c r="F58" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="B59" t="s">
-        <v>274</v>
-      </c>
-      <c r="C59" t="s">
-        <v>38</v>
-      </c>
-      <c r="D59" t="s">
-        <v>43</v>
-      </c>
-      <c r="E59" t="s">
-        <v>44</v>
-      </c>
-      <c r="F59" t="s">
-        <v>292</v>
-      </c>
-    </row>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Updated source code to version 1.0.2
</commit_message>
<xml_diff>
--- a/display-fw/TouchGFX/assets/texts/texts.xlsx
+++ b/display-fw/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24949" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25304" uniqueCount="299">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1062,6 +1062,9 @@
   </si>
   <si>
     <t xml:space="preserve">-., 0123456789CF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: 1.0.2</t>
   </si>
 </sst>
 </file>
@@ -2954,7 +2957,7 @@
         <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="26">

</xml_diff>

<commit_message>
Updated source code to version 1.0.3
</commit_message>
<xml_diff>
--- a/display-fw/TouchGFX/assets/texts/texts.xlsx
+++ b/display-fw/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25304" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25665" uniqueCount="302">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1065,6 +1065,15 @@
   </si>
   <si>
     <t xml:space="preserve">Version: 1.0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: 1.0.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB: &lt;value&gt; °&lt;value&gt;        </t>
   </si>
 </sst>
 </file>
@@ -2957,7 +2966,7 @@
         <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26">
@@ -3521,7 +3530,23 @@
         <v>174</v>
       </c>
     </row>
-    <row r="59"/>
+    <row r="59">
+      <c r="B59" t="s">
+        <v>300</v>
+      </c>
+      <c r="C59" t="s">
+        <v>295</v>
+      </c>
+      <c r="D59" t="s">
+        <v>43</v>
+      </c>
+      <c r="E59" t="s">
+        <v>44</v>
+      </c>
+      <c r="F59" t="s">
+        <v>301</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Updated source code to version 1.0.4
</commit_message>
<xml_diff>
--- a/display-fw/TouchGFX/assets/texts/texts.xlsx
+++ b/display-fw/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25665" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42184" uniqueCount="327">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1074,6 +1074,81 @@
   </si>
   <si>
     <t xml:space="preserve">PCB: &lt;value&gt; °&lt;value&gt;        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CurrentState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current State: &lt;value&gt;     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!-~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"P","r","e","h","a","t","S","o","l","d","i","n","g","t","c"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooling System2: &lt;value&gt; °&lt;value&gt;     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: 1.0.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test </t>
+  </si>
+  <si>
+    <t xml:space="preserve">test&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: 1.5.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State:&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-., 0123456789CF, a-z, A-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-., 0123456789CF, "I", "h"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-., 0123456789CF, "I", "P","r","e","h","a","t","S","o","l","d","i","n","g","t","c","Q","u","k","l"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-., 0123456789CF, "I", "P","r","e","h","a","t","S","o","l","d","i","n","g","t","c","Q","u","k","l","b"</t>
   </si>
 </sst>
 </file>
@@ -2492,7 +2567,7 @@
         <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>297</v>
+        <v>326</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -2954,27 +3029,27 @@
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
         <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>299</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
         <v>43</v>
@@ -2983,49 +3058,49 @@
         <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>215</v>
+        <v>122</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E27" t="s">
         <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>184</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>122</v>
+        <v>220</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
         <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>123</v>
+        <v>258</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D29" t="s">
         <v>43</v>
@@ -3034,15 +3109,15 @@
         <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D30" t="s">
         <v>43</v>
@@ -3051,15 +3126,15 @@
         <v>44</v>
       </c>
       <c r="F30" t="s">
-        <v>269</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D31" t="s">
         <v>43</v>
@@ -3068,12 +3143,12 @@
         <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C32" t="s">
         <v>71</v>
@@ -3085,15 +3160,15 @@
         <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>230</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D33" t="s">
         <v>43</v>
@@ -3107,7 +3182,7 @@
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C34" t="s">
         <v>38</v>
@@ -3124,7 +3199,7 @@
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C35" t="s">
         <v>38</v>
@@ -3136,12 +3211,12 @@
         <v>44</v>
       </c>
       <c r="F35" t="s">
-        <v>57</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C36" t="s">
         <v>38</v>
@@ -3153,12 +3228,12 @@
         <v>44</v>
       </c>
       <c r="F36" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
@@ -3170,12 +3245,12 @@
         <v>44</v>
       </c>
       <c r="F37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C38" t="s">
         <v>38</v>
@@ -3187,12 +3262,12 @@
         <v>44</v>
       </c>
       <c r="F38" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C39" t="s">
         <v>38</v>
@@ -3204,35 +3279,35 @@
         <v>44</v>
       </c>
       <c r="F39" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>244</v>
+        <v>182</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D40" t="s">
-        <v>43</v>
+        <v>143</v>
       </c>
       <c r="E40" t="s">
         <v>44</v>
       </c>
       <c r="F40" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C41" t="s">
         <v>71</v>
       </c>
       <c r="D41" t="s">
-        <v>143</v>
+        <v>43</v>
       </c>
       <c r="E41" t="s">
         <v>44</v>
@@ -3243,41 +3318,41 @@
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>180</v>
+        <v>246</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E42" t="s">
         <v>44</v>
       </c>
       <c r="F42" t="s">
-        <v>181</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C43" t="s">
         <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E43" t="s">
         <v>44</v>
       </c>
       <c r="F43" t="s">
-        <v>123</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
@@ -3289,15 +3364,15 @@
         <v>44</v>
       </c>
       <c r="F44" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C45" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D45" t="s">
         <v>43</v>
@@ -3306,15 +3381,15 @@
         <v>44</v>
       </c>
       <c r="F45" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D46" t="s">
         <v>43</v>
@@ -3323,15 +3398,15 @@
         <v>44</v>
       </c>
       <c r="F46" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C47" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D47" t="s">
         <v>43</v>
@@ -3340,15 +3415,15 @@
         <v>44</v>
       </c>
       <c r="F47" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C48" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D48" t="s">
         <v>43</v>
@@ -3357,15 +3432,15 @@
         <v>44</v>
       </c>
       <c r="F48" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C49" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D49" t="s">
         <v>43</v>
@@ -3374,15 +3449,15 @@
         <v>44</v>
       </c>
       <c r="F49" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D50" t="s">
         <v>43</v>
@@ -3391,15 +3466,15 @@
         <v>44</v>
       </c>
       <c r="F50" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C51" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D51" t="s">
         <v>43</v>
@@ -3408,15 +3483,15 @@
         <v>44</v>
       </c>
       <c r="F51" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C52" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D52" t="s">
         <v>43</v>
@@ -3425,15 +3500,15 @@
         <v>44</v>
       </c>
       <c r="F52" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C53" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D53" t="s">
         <v>43</v>
@@ -3442,15 +3517,15 @@
         <v>44</v>
       </c>
       <c r="F53" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C54" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D54" t="s">
         <v>43</v>
@@ -3459,12 +3534,12 @@
         <v>44</v>
       </c>
       <c r="F54" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C55" t="s">
         <v>38</v>
@@ -3476,12 +3551,12 @@
         <v>44</v>
       </c>
       <c r="F55" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C56" t="s">
         <v>38</v>
@@ -3493,15 +3568,15 @@
         <v>44</v>
       </c>
       <c r="F56" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>274</v>
+        <v>89</v>
       </c>
       <c r="C57" t="s">
-        <v>38</v>
+        <v>295</v>
       </c>
       <c r="D57" t="s">
         <v>43</v>
@@ -3510,12 +3585,12 @@
         <v>44</v>
       </c>
       <c r="F57" t="s">
-        <v>280</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>89</v>
+        <v>300</v>
       </c>
       <c r="C58" t="s">
         <v>295</v>
@@ -3527,26 +3602,46 @@
         <v>44</v>
       </c>
       <c r="F58" t="s">
-        <v>174</v>
+        <v>301</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>300</v>
+        <v>198</v>
       </c>
       <c r="C59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" t="s">
+        <v>50</v>
+      </c>
+      <c r="E59" t="s">
+        <v>44</v>
+      </c>
+      <c r="F59" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>306</v>
+      </c>
+      <c r="C60" t="s">
         <v>295</v>
       </c>
-      <c r="D59" t="s">
-        <v>43</v>
-      </c>
-      <c r="E59" t="s">
-        <v>44</v>
-      </c>
-      <c r="F59" t="s">
-        <v>301</v>
-      </c>
-    </row>
+      <c r="D60" t="s">
+        <v>43</v>
+      </c>
+      <c r="E60" t="s">
+        <v>44</v>
+      </c>
+      <c r="F60" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Updated source code to version 1.0.5
</commit_message>
<xml_diff>
--- a/display-fw/TouchGFX/assets/texts/texts.xlsx
+++ b/display-fw/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42184" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43291" uniqueCount="331">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1149,6 +1149,18 @@
   </si>
   <si>
     <t xml:space="preserve">-., 0123456789CF, "I", "P","r","e","h","a","t","S","o","l","d","i","n","g","t","c","Q","u","k","l","b"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: 1.0.5 beta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: 1.0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_01</t>
   </si>
 </sst>
 </file>
@@ -2589,6 +2601,25 @@
       </c>
     </row>
     <row r="10" spans="2:16">
+      <c r="B10" t="s">
+        <v>329</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10">
+        <v>47</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
       <c r="L10" s="11" t="s">
         <v>28</v>
       </c>
@@ -2604,6 +2635,25 @@
       <c r="P10" s="14"/>
     </row>
     <row r="11" spans="2:16">
+      <c r="B11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:16">
@@ -2692,7 +2742,7 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>329</v>
       </c>
       <c r="D5" t="s">
         <v>43</v>
@@ -3619,7 +3669,7 @@
         <v>44</v>
       </c>
       <c r="F59" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
     </row>
     <row r="60">

</xml_diff>

<commit_message>
optimized code and updated for vapor phase two
</commit_message>
<xml_diff>
--- a/display-fw/TouchGFX/assets/texts/texts.xlsx
+++ b/display-fw/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43291" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44037" uniqueCount="334">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1161,6 +1161,15 @@
   </si>
   <si>
     <t xml:space="preserve">Typography_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vapor Phase Two</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vapor Phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: 1.0.6</t>
   </si>
 </sst>
 </file>
@@ -2751,7 +2760,7 @@
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6">
@@ -3669,7 +3678,7 @@
         <v>44</v>
       </c>
       <c r="F59" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
     </row>
     <row r="60">

</xml_diff>